<commit_message>
update addr files and fixed switch band function
</commit_message>
<xml_diff>
--- a/tc/tc_iot_4/表架拓扑图.xlsx
+++ b/tc/tc_iot_4/表架拓扑图.xlsx
@@ -12,12 +12,11 @@
     <sheet name="线形网络" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="135">
   <si>
     <t>表架1(左侧)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -323,35 +322,239 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>橙色：电表有事件上报，断电再上电，必然会上报</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表架1(左1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表架2（左二）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表架3(左三)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表架4（左四）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>026</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>052</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>059</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粗体：地址开头1809130000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>028</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>036</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>023</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>034</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>025</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>055</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>054</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>058</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>057</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>060</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>051</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>053</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>056</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>046</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>087</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>084</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>035</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>099</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>089</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>097</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>096</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>095</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>094</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>093</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>092</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>019</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -362,7 +565,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +615,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -439,7 +659,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -636,11 +856,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -743,12 +974,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -762,22 +987,91 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1081,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:AB19"/>
+  <dimension ref="C6:AB28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1118,10 +1412,10 @@
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.15">
       <c r="G7" t="s">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="U7" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="3:28" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1139,493 +1433,1031 @@
       <c r="AB8" s="2"/>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.15">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="37">
+        <v>4</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="37">
+        <v>4</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="37">
+        <v>4</v>
+      </c>
+      <c r="I9" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="37">
+        <v>4</v>
+      </c>
+      <c r="K9" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="37">
+        <v>4</v>
+      </c>
+      <c r="M9" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" s="37">
+        <v>4</v>
+      </c>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="R9" s="42">
+        <v>4</v>
+      </c>
+      <c r="S9" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="T9" s="42">
+        <v>4</v>
+      </c>
+      <c r="U9" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="V9" s="42">
+        <v>4</v>
+      </c>
+      <c r="W9" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="X9" s="42">
+        <v>4</v>
+      </c>
+      <c r="Y9" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z9" s="42">
+        <v>4</v>
+      </c>
+      <c r="AA9" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB9" s="42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C10" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="38">
+        <v>5</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="38">
+        <v>5</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="38">
+        <v>5</v>
+      </c>
+      <c r="I10" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="38">
+        <v>5</v>
+      </c>
+      <c r="K10" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="38">
+        <v>5</v>
+      </c>
+      <c r="M10" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="38">
+        <v>5</v>
+      </c>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="R10" s="43">
+        <v>5</v>
+      </c>
+      <c r="S10" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="T10" s="43">
+        <v>5</v>
+      </c>
+      <c r="U10" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="V10" s="43">
+        <v>5</v>
+      </c>
+      <c r="W10" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="X10" s="43">
+        <v>5</v>
+      </c>
+      <c r="Y10" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z10" s="43">
+        <v>5</v>
+      </c>
+      <c r="AA10" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB10" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C11" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="38">
+        <v>4</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="38">
+        <v>4</v>
+      </c>
+      <c r="G11" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="38">
+        <v>4</v>
+      </c>
+      <c r="I11" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="38">
+        <v>4</v>
+      </c>
+      <c r="K11" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="38">
+        <v>4</v>
+      </c>
+      <c r="M11" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="38">
+        <v>4</v>
+      </c>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="R11" s="43">
+        <v>4</v>
+      </c>
+      <c r="S11" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="T11" s="43">
+        <v>4</v>
+      </c>
+      <c r="U11" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="V11" s="43">
+        <v>4</v>
+      </c>
+      <c r="W11" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="X11" s="43">
+        <v>4</v>
+      </c>
+      <c r="Y11" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z11" s="43">
+        <v>4</v>
+      </c>
+      <c r="AA11" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB11" s="43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C12" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="38">
+        <v>2</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="38">
+        <v>2</v>
+      </c>
+      <c r="G12" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="38">
+        <v>2</v>
+      </c>
+      <c r="I12" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="38">
+        <v>2</v>
+      </c>
+      <c r="K12" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="38">
+        <v>2</v>
+      </c>
+      <c r="M12" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="38">
+        <v>2</v>
+      </c>
+      <c r="O12" s="56"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" s="43">
+        <v>2</v>
+      </c>
+      <c r="S12" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="T12" s="43">
+        <v>2</v>
+      </c>
+      <c r="U12" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="V12" s="43">
+        <v>2</v>
+      </c>
+      <c r="W12" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="X12" s="43">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z12" s="43">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB12" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:28" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="39">
+        <v>1</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="39">
+        <v>1</v>
+      </c>
+      <c r="G13" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="39">
+        <v>1</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="39">
+        <v>1</v>
+      </c>
+      <c r="K13" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="39">
+        <v>1</v>
+      </c>
+      <c r="M13" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="39">
+        <v>1</v>
+      </c>
+      <c r="O13" s="56"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="R13" s="44">
+        <v>1</v>
+      </c>
+      <c r="S13" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="T13" s="44">
+        <v>1</v>
+      </c>
+      <c r="U13" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="V13" s="44">
+        <v>1</v>
+      </c>
+      <c r="W13" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="X13" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z13" s="44">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB13" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C14" s="48">
+        <v>0</v>
+      </c>
+      <c r="D14" s="45">
+        <f>SUM(D9:D13)</f>
+        <v>16</v>
+      </c>
+      <c r="E14" s="48">
+        <v>0</v>
+      </c>
+      <c r="F14" s="48">
+        <f>SUM(F9:F13)</f>
+        <v>16</v>
+      </c>
+      <c r="G14" s="48">
+        <v>0</v>
+      </c>
+      <c r="H14" s="48">
+        <f>SUM(H9:H13)</f>
+        <v>16</v>
+      </c>
+      <c r="I14" s="48">
+        <v>0</v>
+      </c>
+      <c r="J14" s="48">
+        <f>SUM(J9:J13)</f>
+        <v>16</v>
+      </c>
+      <c r="K14" s="48">
+        <v>0</v>
+      </c>
+      <c r="L14" s="48">
+        <f>SUM(L9:L13)</f>
+        <v>16</v>
+      </c>
+      <c r="M14" s="48">
+        <v>0</v>
+      </c>
+      <c r="N14" s="48">
+        <f>SUM(N9:N13)</f>
+        <v>16</v>
+      </c>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48">
+        <v>0</v>
+      </c>
+      <c r="R14" s="48">
+        <f>SUM(R9:R13)</f>
+        <v>16</v>
+      </c>
+      <c r="S14" s="48">
+        <v>0</v>
+      </c>
+      <c r="T14" s="48">
+        <f>SUM(T9:T13)</f>
+        <v>16</v>
+      </c>
+      <c r="U14" s="48">
+        <v>0</v>
+      </c>
+      <c r="V14" s="48">
+        <f>SUM(V9:V13)</f>
+        <v>16</v>
+      </c>
+      <c r="W14" s="48">
+        <v>0</v>
+      </c>
+      <c r="X14" s="48">
+        <f>SUM(X9:X13)</f>
+        <v>16</v>
+      </c>
+      <c r="Y14" s="48">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="48">
+        <f>SUM(Z9:Z13)</f>
+        <v>16</v>
+      </c>
+      <c r="AA14" s="48">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="48">
+        <f>SUM(AB9:AB13)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="3:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="V15" s="66"/>
+      <c r="W15" s="49"/>
+      <c r="X15" s="66"/>
+      <c r="Y15" s="49"/>
+      <c r="Z15" s="66"/>
+      <c r="AA15" s="49"/>
+      <c r="AB15" s="67"/>
+    </row>
+    <row r="16" spans="3:28" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="49"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="66"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="66"/>
+      <c r="U16" s="49"/>
+      <c r="V16" s="66"/>
+      <c r="W16" s="49"/>
+      <c r="X16" s="66"/>
+      <c r="Y16" s="49"/>
+      <c r="Z16" s="66"/>
+      <c r="AA16" s="49"/>
+      <c r="AB16" s="66"/>
+    </row>
+    <row r="17" spans="3:28" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="42">
+        <v>5</v>
+      </c>
+      <c r="E17" s="69" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="42">
+        <v>5</v>
+      </c>
+      <c r="G17" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="42">
+        <v>5</v>
+      </c>
+      <c r="I17" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="42">
+        <v>5</v>
+      </c>
+      <c r="K17" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17" s="42">
+        <v>5</v>
+      </c>
+      <c r="M17" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="N17" s="42">
+        <v>5</v>
+      </c>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="R17" s="42">
+        <v>5</v>
+      </c>
+      <c r="S17" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="T17" s="42">
+        <v>5</v>
+      </c>
+      <c r="U17" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="V17" s="42">
+        <v>5</v>
+      </c>
+      <c r="W17" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="X17" s="42">
+        <v>5</v>
+      </c>
+      <c r="Y17" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z17" s="42">
+        <v>5</v>
+      </c>
+      <c r="AA17" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB17" s="42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:28" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="43">
+        <v>4</v>
+      </c>
+      <c r="E18" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="43">
+        <v>4</v>
+      </c>
+      <c r="G18" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="43">
+        <v>4</v>
+      </c>
+      <c r="I18" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="43">
+        <v>4</v>
+      </c>
+      <c r="K18" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="43">
+        <v>4</v>
+      </c>
+      <c r="M18" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="N18" s="43">
+        <v>4</v>
+      </c>
+      <c r="O18" s="56"/>
+      <c r="P18" s="56"/>
+      <c r="Q18" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="R18" s="43">
+        <v>4</v>
+      </c>
+      <c r="S18" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="T18" s="43">
+        <v>4</v>
+      </c>
+      <c r="U18" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="V18" s="43">
+        <v>4</v>
+      </c>
+      <c r="W18" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="X18" s="43">
+        <v>4</v>
+      </c>
+      <c r="Y18" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z18" s="43">
+        <v>4</v>
+      </c>
+      <c r="AA18" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB18" s="43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C19" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="43">
+        <v>3</v>
+      </c>
+      <c r="E19" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="43">
+        <v>3</v>
+      </c>
+      <c r="G19" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="43">
+        <v>3</v>
+      </c>
+      <c r="I19" s="71" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="43">
+        <v>3</v>
+      </c>
+      <c r="K19" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="L19" s="43">
+        <v>3</v>
+      </c>
+      <c r="M19" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="N19" s="43">
+        <v>3</v>
+      </c>
+      <c r="O19" s="56"/>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="R19" s="43">
+        <v>3</v>
+      </c>
+      <c r="S19" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="T19" s="43">
+        <v>3</v>
+      </c>
+      <c r="U19" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="V19" s="43">
+        <v>3</v>
+      </c>
+      <c r="W19" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="X19" s="43">
+        <v>3</v>
+      </c>
+      <c r="Y19" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z19" s="43">
+        <v>3</v>
+      </c>
+      <c r="AA19" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB19" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:28" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="43">
+        <v>2</v>
+      </c>
+      <c r="E20" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="43">
+        <v>2</v>
+      </c>
+      <c r="G20" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="43">
+        <v>2</v>
+      </c>
+      <c r="I20" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="J20" s="43">
+        <v>2</v>
+      </c>
+      <c r="K20" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="L20" s="43">
+        <v>2</v>
+      </c>
+      <c r="M20" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="N20" s="43">
+        <v>2</v>
+      </c>
+      <c r="O20" s="56"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="R20" s="43">
+        <v>2</v>
+      </c>
+      <c r="S20" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="T20" s="43">
+        <v>2</v>
+      </c>
+      <c r="U20" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="V20" s="43">
+        <v>2</v>
+      </c>
+      <c r="W20" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="X20" s="43">
+        <v>2</v>
+      </c>
+      <c r="Y20" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z20" s="43">
+        <v>2</v>
+      </c>
+      <c r="AA20" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB20" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:28" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="44">
+        <v>1</v>
+      </c>
+      <c r="E21" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="44">
+        <v>1</v>
+      </c>
+      <c r="G21" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="44">
+        <v>1</v>
+      </c>
+      <c r="I21" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21" s="44">
+        <v>1</v>
+      </c>
+      <c r="K21" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="L21" s="44">
+        <v>1</v>
+      </c>
+      <c r="M21" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="N21" s="44">
+        <v>1</v>
+      </c>
+      <c r="O21" s="56"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="R21" s="44">
+        <v>1</v>
+      </c>
+      <c r="S21" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="T21" s="44">
+        <v>1</v>
+      </c>
+      <c r="U21" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="V21" s="44">
+        <v>1</v>
+      </c>
+      <c r="W21" s="62" t="s">
+        <v>111</v>
+      </c>
+      <c r="X21" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z21" s="44">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB21" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="D22" s="36">
+        <f>SUM(D17:D21)</f>
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <f>SUM(F17:F21)</f>
+        <v>15</v>
+      </c>
+      <c r="H22">
+        <f>SUM(H17:H21)</f>
+        <v>15</v>
+      </c>
+      <c r="J22">
+        <f>SUM(J17:J21)</f>
+        <v>15</v>
+      </c>
+      <c r="L22">
+        <f>SUM(L17:L21)</f>
+        <v>15</v>
+      </c>
+      <c r="N22">
+        <f>SUM(N17:N21)</f>
+        <v>15</v>
+      </c>
+      <c r="R22">
+        <f>SUM(R17:R21)</f>
+        <v>15</v>
+      </c>
+      <c r="T22">
+        <f>SUM(T17:T21)</f>
+        <v>15</v>
+      </c>
+      <c r="V22">
+        <f>SUM(V17:V21)</f>
+        <v>15</v>
+      </c>
+      <c r="X22">
+        <f>SUM(X17:X21)</f>
+        <v>15</v>
+      </c>
+      <c r="Z22">
+        <f>SUM(Z17:Z21)</f>
+        <v>15</v>
+      </c>
+      <c r="AB22">
+        <f>SUM(AB17:AB21)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="R23"/>
+      <c r="T23"/>
+      <c r="V23"/>
+      <c r="X23"/>
+      <c r="Z23"/>
+      <c r="AB23" s="36"/>
+    </row>
+    <row r="24" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C24" t="s">
+        <v>62</v>
+      </c>
+      <c r="R24"/>
+      <c r="T24"/>
+      <c r="V24"/>
+      <c r="X24"/>
+      <c r="Z24"/>
+      <c r="AB24" s="36">
+        <f>SUM(D22:AB22)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="R25"/>
+      <c r="T25"/>
+      <c r="V25"/>
+      <c r="X25"/>
+      <c r="Z25"/>
+      <c r="AB25" s="36">
+        <f>SUM(D14:AB14)</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="R26"/>
+      <c r="T26"/>
+      <c r="V26"/>
+      <c r="X26"/>
+      <c r="Z26"/>
+      <c r="AB26"/>
+    </row>
+    <row r="27" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C27" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L9" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="N9" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="R9" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="S9" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="T9" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="U9" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="V9" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="W9" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="X9" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y9" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z9" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA9" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB9" s="39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="3:28" x14ac:dyDescent="0.15">
-      <c r="C10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="N10" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="R10" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="S10" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="T10" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="U10" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="V10" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="W10" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="X10" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y10" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z10" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA10" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB10" s="40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="3:28" x14ac:dyDescent="0.15">
-      <c r="C11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="K11" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="R11" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="S11" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="T11" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="U11" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="V11" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="W11" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="X11" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y11" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z11" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA11" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB11" s="40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="3:28" x14ac:dyDescent="0.15">
-      <c r="C12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="R12" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="S12" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="T12" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="U12" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="V12" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="W12" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="X12" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y12" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z12" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA12" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB12" s="40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="3:28" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="K13" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="R13" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="S13" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="T13" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="U13" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="V13" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="W13" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="X13" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y13" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z13" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA13" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB13" s="41" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="3:28" x14ac:dyDescent="0.15">
-      <c r="D14" s="38">
-        <f>SUM(D9:D13)</f>
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <f>SUM(F9:F13)</f>
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <f>SUM(H9:H13)</f>
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <f>SUM(J9:J13)</f>
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <f>SUM(L9:L13)</f>
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <f>SUM(N9:N13)</f>
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <f>SUM(R9:R13)</f>
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <f>SUM(T9:T13)</f>
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <f>SUM(V9:V13)</f>
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <f>SUM(X9:X13)</f>
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <f>SUM(Z9:Z13)</f>
-        <v>0</v>
-      </c>
-      <c r="AB14">
-        <f>SUM(AB9:AB13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="3:28" x14ac:dyDescent="0.15">
-      <c r="R15"/>
-      <c r="T15"/>
-      <c r="V15"/>
-      <c r="X15"/>
-      <c r="Z15"/>
-      <c r="AB15"/>
-    </row>
-    <row r="16" spans="3:28" x14ac:dyDescent="0.15">
-      <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="R16"/>
-      <c r="T16"/>
-      <c r="V16"/>
-      <c r="X16"/>
-      <c r="Z16"/>
-      <c r="AB16"/>
-    </row>
-    <row r="17" spans="3:28" x14ac:dyDescent="0.15">
-      <c r="C17" t="s">
-        <v>63</v>
-      </c>
-      <c r="R17"/>
-      <c r="T17"/>
-      <c r="V17"/>
-      <c r="X17"/>
-      <c r="Z17"/>
-      <c r="AB17"/>
-    </row>
-    <row r="18" spans="3:28" x14ac:dyDescent="0.15">
-      <c r="C18" t="s">
-        <v>64</v>
-      </c>
-      <c r="R18"/>
-      <c r="T18"/>
-      <c r="V18"/>
-      <c r="X18"/>
-      <c r="Z18"/>
-      <c r="AB18"/>
-    </row>
-    <row r="19" spans="3:28" x14ac:dyDescent="0.15">
-      <c r="C19" t="s">
-        <v>83</v>
-      </c>
-      <c r="R19"/>
-      <c r="T19"/>
-      <c r="V19"/>
-      <c r="X19"/>
-      <c r="Z19"/>
-      <c r="AB19"/>
+      <c r="R27"/>
+      <c r="T27"/>
+      <c r="V27"/>
+      <c r="X27"/>
+      <c r="Z27"/>
+      <c r="AB27"/>
+    </row>
+    <row r="28" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C9 C13 C12 C11 C10 E10 G10 I10 K10 M10 O10:Q10 O9:Q9 M9 K9 I9 G9 E9 E11 G11 I11 K11 M11 O11:Q11 AA9 Y9 W9 U9 S9 S10 U10 W10 Y10 AA10 AA11 Y11 W11 U11 S11 S12 U12 W12 Y12 AA12 D12:Q12 AA13 Y13 W13 U13 S13 D13:Q13 D9 R13 T13 V13 X13 Z13 AB13 R12 AB12 Z12 X12 V12 T12 D11 T11 V11 X11 Z11 AB11 D10 AB10 Z10 X10 V10 T10 T9 V9 X9 Z9 AB9 R11 N11 L11 J11 H11 F11 F9 H9 J9 L9 N9 R9 R10 N10 L10 J10 H10 F10" numberStoredAsText="1"/>
+    <ignoredError sqref="C9 C13 C12 C11 C10 E10 G10 I10 K10 M10 O10:Q10 O9:Q9 M9 K9 I9 G9 E9 E11 G11 I11 K11 M11 O11:Q11 AA9 Y9 W9 U9 S9 S10 U10 W10 Y10 AA10 AA11 Y11 W11 U11 S11 S12 U12 W12 Y12 AA12 E12 AA13 Y13 W13 U13 S13 E13 G12 G13 I12 I13 K12 K13 M12 M13 O12:Q12 O13:Q13 O19:P19 O20:P20 O21:P21 O17:P17 O18:P18 C18 C17 C20 C19 G20 C22:N22 C21 E21 I20 K20 M20 I21 K21 M21 AB21 Z21 X21 V21 T21 R21 AB20 Z20 X20 V20 T20 R20 AB19 Z19 X19 V19 T19 R19 AB18 Z18 X18 V18 T18 R18 AB17 Z17 X17 V17 T17 R17 Q22:AB22 Q17 S17 U17 W17 Y17 AA17 Q18 S18 U18 W18 Y18 AA18 Q19 S19 U19 W19 Y19 AA19 Q20 S20 U20 W20 Y20 AA20 Q21 S21 U21 W21 Y21 AA21 E18 E17 E20 E19 G21 G18 G17 G19 I18 I17 I19 K18 K17 K19 M18 M17 M19" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2116,7 +2948,7 @@
   <dimension ref="C9:AB20"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>